<commit_message>
Refactor tournament registration process and improve logging
- Updated comments for clarity in the main.py file.
- Enhanced error handling during the registration process, providing more informative logging.
- Improved the flow of the registration logic, ensuring proper handling of both unregister and register buttons.
- Added sleep intervals to manage timing issues during button interactions.
- Updated the accounts_MAIN.xlsx file to reflect recent changes in data management.
</commit_message>
<xml_diff>
--- a/accounts_MAIN.xlsx
+++ b/accounts_MAIN.xlsx
@@ -497,23 +497,13 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10.000 TL Omaha4 Ücretsiz Turnuva</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2024-11-27 23:13:43</t>
-        </is>
-      </c>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -527,8 +517,14 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -547,21 +543,15 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2024-11-27 23:14:20</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -576,7 +566,11 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
@@ -595,7 +589,11 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -614,7 +612,11 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
@@ -633,7 +635,11 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
@@ -652,7 +658,11 @@
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
@@ -671,7 +681,11 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
@@ -690,7 +704,11 @@
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
@@ -709,7 +727,11 @@
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
@@ -727,22 +749,18 @@
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>2024-11-27 23:13:43</t>
-        </is>
-      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -757,7 +775,11 @@
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
@@ -776,7 +798,11 @@
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
@@ -795,7 +821,11 @@
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
@@ -814,7 +844,11 @@
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
@@ -833,7 +867,11 @@
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
@@ -852,7 +890,11 @@
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
@@ -871,7 +913,11 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -890,7 +936,11 @@
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
@@ -909,7 +959,11 @@
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
@@ -928,7 +982,11 @@
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
@@ -947,7 +1005,11 @@
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
@@ -966,7 +1028,11 @@
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
@@ -985,7 +1051,11 @@
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
@@ -1004,7 +1074,11 @@
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
@@ -1023,7 +1097,11 @@
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
@@ -1042,7 +1120,11 @@
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
@@ -1061,7 +1143,11 @@
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
@@ -1079,8 +1165,14 @@
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
@@ -1099,7 +1191,11 @@
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>10.000 TL Texas Ücretsiz Turnuva</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>

</xml_diff>